<commit_message>
daily auto push: 2025-09-03 13:35 UTC
</commit_message>
<xml_diff>
--- a/excel/spotify.xlsx
+++ b/excel/spotify.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D559"/>
+  <dimension ref="A1:D560"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10499,6 +10499,24 @@
         <v>101</v>
       </c>
     </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>2025/09/02</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>火</t>
+        </is>
+      </c>
+      <c r="C560" t="n">
+        <v>21</v>
+      </c>
+      <c r="D560" t="n">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
daily auto push: 2025-09-09 02:02 UTC
</commit_message>
<xml_diff>
--- a/excel/spotify.xlsx
+++ b/excel/spotify.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D562"/>
+  <dimension ref="A1:D563"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10553,6 +10553,24 @@
         <v>101</v>
       </c>
     </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>2025/09/05</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>金</t>
+        </is>
+      </c>
+      <c r="C563" t="n">
+        <v>21</v>
+      </c>
+      <c r="D563" t="n">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
daily auto push: 2025-10-11 13:28 UTC
</commit_message>
<xml_diff>
--- a/excel/spotify.xlsx
+++ b/excel/spotify.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D595"/>
+  <dimension ref="A1:D596"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11147,6 +11147,24 @@
         <v>101</v>
       </c>
     </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>2025/10/10</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>金</t>
+        </is>
+      </c>
+      <c r="C596" t="n">
+        <v>21</v>
+      </c>
+      <c r="D596" t="n">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
daily auto push: 2025-10-31 13:38 UTC
</commit_message>
<xml_diff>
--- a/excel/spotify.xlsx
+++ b/excel/spotify.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D615"/>
+  <dimension ref="A1:D616"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11507,6 +11507,24 @@
         <v>101</v>
       </c>
     </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>2025/10/30</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>木</t>
+        </is>
+      </c>
+      <c r="C616" t="n">
+        <v>21</v>
+      </c>
+      <c r="D616" t="n">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
daily auto push: 2025-12-08 22:33 UTC
</commit_message>
<xml_diff>
--- a/excel/spotify.xlsx
+++ b/excel/spotify.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D653"/>
+  <dimension ref="A1:D654"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12191,6 +12191,24 @@
         <v>101</v>
       </c>
     </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>2025/12/07</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>日</t>
+        </is>
+      </c>
+      <c r="C654" t="n">
+        <v>22</v>
+      </c>
+      <c r="D654" t="n">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
daily auto push: 2025-12-09 13:46 UTC
</commit_message>
<xml_diff>
--- a/excel/spotify.xlsx
+++ b/excel/spotify.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D654"/>
+  <dimension ref="A1:D655"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12209,6 +12209,24 @@
         <v>101</v>
       </c>
     </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>2025/12/09</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>火</t>
+        </is>
+      </c>
+      <c r="C655" t="n">
+        <v>4</v>
+      </c>
+      <c r="D655" t="n">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
daily auto push: 2025-12-11 22:34 UTC
</commit_message>
<xml_diff>
--- a/excel/spotify.xlsx
+++ b/excel/spotify.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D656"/>
+  <dimension ref="A1:D657"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12245,6 +12245,24 @@
         <v>101</v>
       </c>
     </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>2025/12/10</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>水</t>
+        </is>
+      </c>
+      <c r="C657" t="n">
+        <v>22</v>
+      </c>
+      <c r="D657" t="n">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
daily auto push: 2025-12-16 13:48 UTC
</commit_message>
<xml_diff>
--- a/excel/spotify.xlsx
+++ b/excel/spotify.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D661"/>
+  <dimension ref="A1:D662"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12335,6 +12335,24 @@
         <v>101</v>
       </c>
     </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>2025/12/15</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>月</t>
+        </is>
+      </c>
+      <c r="C662" t="n">
+        <v>22</v>
+      </c>
+      <c r="D662" t="n">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
daily auto push: 2025-12-20 13:35 UTC
</commit_message>
<xml_diff>
--- a/excel/spotify.xlsx
+++ b/excel/spotify.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D665"/>
+  <dimension ref="A1:D666"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12407,6 +12407,24 @@
         <v>101</v>
       </c>
     </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>2025/12/19</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>金</t>
+        </is>
+      </c>
+      <c r="C666" t="n">
+        <v>22</v>
+      </c>
+      <c r="D666" t="n">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
daily auto push: 2025-12-28 13:37 UTC
</commit_message>
<xml_diff>
--- a/excel/spotify.xlsx
+++ b/excel/spotify.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D673"/>
+  <dimension ref="A1:D674"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12551,6 +12551,24 @@
         <v>101</v>
       </c>
     </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>2025/12/27</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>土</t>
+        </is>
+      </c>
+      <c r="C674" t="n">
+        <v>23</v>
+      </c>
+      <c r="D674" t="n">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
daily auto push: 2025-12-30 13:46 UTC
</commit_message>
<xml_diff>
--- a/excel/spotify.xlsx
+++ b/excel/spotify.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D675"/>
+  <dimension ref="A1:D676"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12587,6 +12587,24 @@
         <v>101</v>
       </c>
     </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>2025/12/29</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>月</t>
+        </is>
+      </c>
+      <c r="C676" t="n">
+        <v>22</v>
+      </c>
+      <c r="D676" t="n">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
daily auto push: 2025-12-31 13:42 UTC
</commit_message>
<xml_diff>
--- a/excel/spotify.xlsx
+++ b/excel/spotify.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D676"/>
+  <dimension ref="A1:D677"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12605,6 +12605,24 @@
         <v>101</v>
       </c>
     </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>2025/12/30</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>火</t>
+        </is>
+      </c>
+      <c r="C677" t="n">
+        <v>22</v>
+      </c>
+      <c r="D677" t="n">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
daily auto push: 2026-01-01 13:43 UTC
</commit_message>
<xml_diff>
--- a/excel/spotify.xlsx
+++ b/excel/spotify.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D677"/>
+  <dimension ref="A1:D678"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12623,6 +12623,24 @@
         <v>101</v>
       </c>
     </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>2025/12/31</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>水</t>
+        </is>
+      </c>
+      <c r="C678" t="n">
+        <v>22</v>
+      </c>
+      <c r="D678" t="n">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
daily auto push: 2026-01-23 13:51 UTC
</commit_message>
<xml_diff>
--- a/excel/spotify.xlsx
+++ b/excel/spotify.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D705"/>
+  <dimension ref="A1:D706"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13022,12 +13022,12 @@
     <row r="700">
       <c r="A700" t="inlineStr">
         <is>
-          <t>2026/12/29</t>
+          <t>2026/01/22</t>
         </is>
       </c>
       <c r="B700" t="inlineStr">
         <is>
-          <t>火</t>
+          <t>木</t>
         </is>
       </c>
       <c r="C700" t="n">
@@ -13040,12 +13040,12 @@
     <row r="701">
       <c r="A701" t="inlineStr">
         <is>
-          <t>2026/12/30</t>
+          <t>2026/12/29</t>
         </is>
       </c>
       <c r="B701" t="inlineStr">
         <is>
-          <t>水</t>
+          <t>火</t>
         </is>
       </c>
       <c r="C701" t="n">
@@ -13058,12 +13058,12 @@
     <row r="702">
       <c r="A702" t="inlineStr">
         <is>
-          <t>2026/12/31</t>
+          <t>2026/12/30</t>
         </is>
       </c>
       <c r="B702" t="inlineStr">
         <is>
-          <t>木</t>
+          <t>水</t>
         </is>
       </c>
       <c r="C702" t="n">
@@ -13076,12 +13076,12 @@
     <row r="703">
       <c r="A703" t="inlineStr">
         <is>
-          <t>2027/01/01</t>
+          <t>2026/12/31</t>
         </is>
       </c>
       <c r="B703" t="inlineStr">
         <is>
-          <t>金</t>
+          <t>木</t>
         </is>
       </c>
       <c r="C703" t="n">
@@ -13094,12 +13094,12 @@
     <row r="704">
       <c r="A704" t="inlineStr">
         <is>
-          <t>2027/01/02</t>
+          <t>2027/01/01</t>
         </is>
       </c>
       <c r="B704" t="inlineStr">
         <is>
-          <t>土</t>
+          <t>金</t>
         </is>
       </c>
       <c r="C704" t="n">
@@ -13112,18 +13112,36 @@
     <row r="705">
       <c r="A705" t="inlineStr">
         <is>
+          <t>2027/01/02</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>土</t>
+        </is>
+      </c>
+      <c r="C705" t="n">
+        <v>22</v>
+      </c>
+      <c r="D705" t="n">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
           <t>2027/01/03</t>
         </is>
       </c>
-      <c r="B705" t="inlineStr">
+      <c r="B706" t="inlineStr">
         <is>
           <t>日</t>
         </is>
       </c>
-      <c r="C705" t="n">
-        <v>22</v>
-      </c>
-      <c r="D705" t="n">
+      <c r="C706" t="n">
+        <v>22</v>
+      </c>
+      <c r="D706" t="n">
         <v>101</v>
       </c>
     </row>

</xml_diff>

<commit_message>
daily auto push: 2026-02-17 14:11 UTC
</commit_message>
<xml_diff>
--- a/excel/spotify.xlsx
+++ b/excel/spotify.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D730"/>
+  <dimension ref="A1:D731"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13472,12 +13472,12 @@
     <row r="725">
       <c r="A725" t="inlineStr">
         <is>
-          <t>2026/12/29</t>
+          <t>2026/02/16</t>
         </is>
       </c>
       <c r="B725" t="inlineStr">
         <is>
-          <t>火</t>
+          <t>月</t>
         </is>
       </c>
       <c r="C725" t="n">
@@ -13490,12 +13490,12 @@
     <row r="726">
       <c r="A726" t="inlineStr">
         <is>
-          <t>2026/12/30</t>
+          <t>2026/12/29</t>
         </is>
       </c>
       <c r="B726" t="inlineStr">
         <is>
-          <t>水</t>
+          <t>火</t>
         </is>
       </c>
       <c r="C726" t="n">
@@ -13508,12 +13508,12 @@
     <row r="727">
       <c r="A727" t="inlineStr">
         <is>
-          <t>2026/12/31</t>
+          <t>2026/12/30</t>
         </is>
       </c>
       <c r="B727" t="inlineStr">
         <is>
-          <t>木</t>
+          <t>水</t>
         </is>
       </c>
       <c r="C727" t="n">
@@ -13526,12 +13526,12 @@
     <row r="728">
       <c r="A728" t="inlineStr">
         <is>
-          <t>2027/01/01</t>
+          <t>2026/12/31</t>
         </is>
       </c>
       <c r="B728" t="inlineStr">
         <is>
-          <t>金</t>
+          <t>木</t>
         </is>
       </c>
       <c r="C728" t="n">
@@ -13544,12 +13544,12 @@
     <row r="729">
       <c r="A729" t="inlineStr">
         <is>
-          <t>2027/01/02</t>
+          <t>2027/01/01</t>
         </is>
       </c>
       <c r="B729" t="inlineStr">
         <is>
-          <t>土</t>
+          <t>金</t>
         </is>
       </c>
       <c r="C729" t="n">
@@ -13562,18 +13562,36 @@
     <row r="730">
       <c r="A730" t="inlineStr">
         <is>
+          <t>2027/01/02</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>土</t>
+        </is>
+      </c>
+      <c r="C730" t="n">
+        <v>22</v>
+      </c>
+      <c r="D730" t="n">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
           <t>2027/01/03</t>
         </is>
       </c>
-      <c r="B730" t="inlineStr">
+      <c r="B731" t="inlineStr">
         <is>
           <t>日</t>
         </is>
       </c>
-      <c r="C730" t="n">
-        <v>22</v>
-      </c>
-      <c r="D730" t="n">
+      <c r="C731" t="n">
+        <v>22</v>
+      </c>
+      <c r="D731" t="n">
         <v>101</v>
       </c>
     </row>

</xml_diff>

<commit_message>
daily auto push: 2026-02-18 05:03 UTC
</commit_message>
<xml_diff>
--- a/excel/spotify.xlsx
+++ b/excel/spotify.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D731"/>
+  <dimension ref="A1:D732"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13490,7 +13490,7 @@
     <row r="726">
       <c r="A726" t="inlineStr">
         <is>
-          <t>2026/12/29</t>
+          <t>2026/02/17</t>
         </is>
       </c>
       <c r="B726" t="inlineStr">
@@ -13508,12 +13508,12 @@
     <row r="727">
       <c r="A727" t="inlineStr">
         <is>
-          <t>2026/12/30</t>
+          <t>2026/12/29</t>
         </is>
       </c>
       <c r="B727" t="inlineStr">
         <is>
-          <t>水</t>
+          <t>火</t>
         </is>
       </c>
       <c r="C727" t="n">
@@ -13526,12 +13526,12 @@
     <row r="728">
       <c r="A728" t="inlineStr">
         <is>
-          <t>2026/12/31</t>
+          <t>2026/12/30</t>
         </is>
       </c>
       <c r="B728" t="inlineStr">
         <is>
-          <t>木</t>
+          <t>水</t>
         </is>
       </c>
       <c r="C728" t="n">
@@ -13544,12 +13544,12 @@
     <row r="729">
       <c r="A729" t="inlineStr">
         <is>
-          <t>2027/01/01</t>
+          <t>2026/12/31</t>
         </is>
       </c>
       <c r="B729" t="inlineStr">
         <is>
-          <t>金</t>
+          <t>木</t>
         </is>
       </c>
       <c r="C729" t="n">
@@ -13562,12 +13562,12 @@
     <row r="730">
       <c r="A730" t="inlineStr">
         <is>
-          <t>2027/01/02</t>
+          <t>2027/01/01</t>
         </is>
       </c>
       <c r="B730" t="inlineStr">
         <is>
-          <t>土</t>
+          <t>金</t>
         </is>
       </c>
       <c r="C730" t="n">
@@ -13580,18 +13580,36 @@
     <row r="731">
       <c r="A731" t="inlineStr">
         <is>
+          <t>2027/01/02</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>土</t>
+        </is>
+      </c>
+      <c r="C731" t="n">
+        <v>22</v>
+      </c>
+      <c r="D731" t="n">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
           <t>2027/01/03</t>
         </is>
       </c>
-      <c r="B731" t="inlineStr">
+      <c r="B732" t="inlineStr">
         <is>
           <t>日</t>
         </is>
       </c>
-      <c r="C731" t="n">
-        <v>22</v>
-      </c>
-      <c r="D731" t="n">
+      <c r="C732" t="n">
+        <v>22</v>
+      </c>
+      <c r="D732" t="n">
         <v>101</v>
       </c>
     </row>

</xml_diff>

<commit_message>
daily auto push: 2026-02-18 14:11 UTC
</commit_message>
<xml_diff>
--- a/excel/spotify.xlsx
+++ b/excel/spotify.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D732"/>
+  <dimension ref="A1:D733"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13508,16 +13508,16 @@
     <row r="727">
       <c r="A727" t="inlineStr">
         <is>
-          <t>2026/12/29</t>
+          <t>2026/02/18</t>
         </is>
       </c>
       <c r="B727" t="inlineStr">
         <is>
-          <t>火</t>
+          <t>水</t>
         </is>
       </c>
       <c r="C727" t="n">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="D727" t="n">
         <v>101</v>
@@ -13526,12 +13526,12 @@
     <row r="728">
       <c r="A728" t="inlineStr">
         <is>
-          <t>2026/12/30</t>
+          <t>2026/12/29</t>
         </is>
       </c>
       <c r="B728" t="inlineStr">
         <is>
-          <t>水</t>
+          <t>火</t>
         </is>
       </c>
       <c r="C728" t="n">
@@ -13544,12 +13544,12 @@
     <row r="729">
       <c r="A729" t="inlineStr">
         <is>
-          <t>2026/12/31</t>
+          <t>2026/12/30</t>
         </is>
       </c>
       <c r="B729" t="inlineStr">
         <is>
-          <t>木</t>
+          <t>水</t>
         </is>
       </c>
       <c r="C729" t="n">
@@ -13562,12 +13562,12 @@
     <row r="730">
       <c r="A730" t="inlineStr">
         <is>
-          <t>2027/01/01</t>
+          <t>2026/12/31</t>
         </is>
       </c>
       <c r="B730" t="inlineStr">
         <is>
-          <t>金</t>
+          <t>木</t>
         </is>
       </c>
       <c r="C730" t="n">
@@ -13580,12 +13580,12 @@
     <row r="731">
       <c r="A731" t="inlineStr">
         <is>
-          <t>2027/01/02</t>
+          <t>2027/01/01</t>
         </is>
       </c>
       <c r="B731" t="inlineStr">
         <is>
-          <t>土</t>
+          <t>金</t>
         </is>
       </c>
       <c r="C731" t="n">
@@ -13598,18 +13598,36 @@
     <row r="732">
       <c r="A732" t="inlineStr">
         <is>
+          <t>2027/01/02</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>土</t>
+        </is>
+      </c>
+      <c r="C732" t="n">
+        <v>22</v>
+      </c>
+      <c r="D732" t="n">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
           <t>2027/01/03</t>
         </is>
       </c>
-      <c r="B732" t="inlineStr">
+      <c r="B733" t="inlineStr">
         <is>
           <t>日</t>
         </is>
       </c>
-      <c r="C732" t="n">
-        <v>22</v>
-      </c>
-      <c r="D732" t="n">
+      <c r="C733" t="n">
+        <v>22</v>
+      </c>
+      <c r="D733" t="n">
         <v>101</v>
       </c>
     </row>

</xml_diff>